<commit_message>
updated scripts for the taxaplots
</commit_message>
<xml_diff>
--- a/phylogenetic_trees/Seaview/diatoms_in_18S_data.xlsx
+++ b/phylogenetic_trees/Seaview/diatoms_in_18S_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreajackman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreajackman/R_Stuff/Parfrey/MH_diatoms_metadata_and_scripts/phylogenetic_trees/Seaview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD9CFC-1B0E-BF46-8637-74CD8DA40F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42B41ED8-BFEC-0541-92C5-1E73C7C9F18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="520" windowWidth="28040" windowHeight="16580" xr2:uid="{067135B1-F6F0-6B43-A6A7-FFABF057F496}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="647">
   <si>
     <t>seq</t>
   </si>
@@ -1971,6 +1971,9 @@
   </si>
   <si>
     <t>Cocconeis_sister</t>
+  </si>
+  <si>
+    <t>Chaetocerotales</t>
   </si>
 </sst>
 </file>
@@ -2472,11 +2475,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2853,11 +2855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DB6B71-5237-4048-B4EA-F1AE145FDAAC}">
-  <dimension ref="A1:P263"/>
+  <dimension ref="A1:O261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="760" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomLeft" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2866,7 +2868,7 @@
     <col min="14" max="14" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2913,7 +2915,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2959,9 +2961,8 @@
       <c r="O2" t="s">
         <v>643</v>
       </c>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3004,9 +3005,8 @@
       <c r="O3" t="s">
         <v>643</v>
       </c>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3052,9 +3052,8 @@
       <c r="O4" t="s">
         <v>643</v>
       </c>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3088,9 +3087,8 @@
       <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -3124,9 +3122,8 @@
       <c r="N6" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -3160,9 +3157,8 @@
       <c r="N7" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3196,9 +3192,8 @@
       <c r="N8" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -3232,9 +3227,8 @@
       <c r="N9" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3268,9 +3262,8 @@
       <c r="N10" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -3304,9 +3297,8 @@
       <c r="N11" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -3352,9 +3344,8 @@
       <c r="O12" t="s">
         <v>643</v>
       </c>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -3400,9 +3391,8 @@
       <c r="O13" t="s">
         <v>643</v>
       </c>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -3448,9 +3438,8 @@
       <c r="O14" t="s">
         <v>643</v>
       </c>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3496,9 +3485,8 @@
       <c r="O15" t="s">
         <v>643</v>
       </c>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -3544,9 +3532,8 @@
       <c r="O16" t="s">
         <v>643</v>
       </c>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -3592,9 +3579,8 @@
       <c r="O17" t="s">
         <v>643</v>
       </c>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3637,9 +3623,8 @@
       <c r="O18" t="s">
         <v>643</v>
       </c>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -3685,9 +3670,8 @@
       <c r="O19" t="s">
         <v>643</v>
       </c>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -3730,9 +3714,8 @@
       <c r="O20" t="s">
         <v>643</v>
       </c>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -3775,9 +3758,8 @@
       <c r="O21" t="s">
         <v>643</v>
       </c>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>157</v>
       </c>
@@ -3823,9 +3805,8 @@
       <c r="O22" t="s">
         <v>643</v>
       </c>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -3868,9 +3849,8 @@
       <c r="O23" t="s">
         <v>643</v>
       </c>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -3904,9 +3884,8 @@
       <c r="N24" t="s">
         <v>79</v>
       </c>
-      <c r="P24" s="3"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>161</v>
       </c>
@@ -3940,9 +3919,8 @@
       <c r="N25" t="s">
         <v>162</v>
       </c>
-      <c r="P25" s="3"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>164</v>
       </c>
@@ -3976,9 +3954,8 @@
       <c r="N26" t="s">
         <v>162</v>
       </c>
-      <c r="P26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>166</v>
       </c>
@@ -4012,9 +3989,8 @@
       <c r="N27" t="s">
         <v>162</v>
       </c>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -4048,9 +4024,8 @@
       <c r="N28" t="s">
         <v>162</v>
       </c>
-      <c r="P28" s="3"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>457</v>
       </c>
@@ -4084,9 +4059,8 @@
       <c r="N29" t="s">
         <v>441</v>
       </c>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>503</v>
       </c>
@@ -4124,7 +4098,7 @@
         <v>85</v>
       </c>
       <c r="M30" t="s">
-        <v>81</v>
+        <v>646</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>644</v>
@@ -4132,9 +4106,8 @@
       <c r="O30" t="s">
         <v>643</v>
       </c>
-      <c r="P30" s="3"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>506</v>
       </c>
@@ -4168,9 +4141,8 @@
       <c r="N31" t="s">
         <v>85</v>
       </c>
-      <c r="P31" s="3"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>508</v>
       </c>
@@ -4204,9 +4176,8 @@
       <c r="N32" t="s">
         <v>85</v>
       </c>
-      <c r="P32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>512</v>
       </c>
@@ -4240,9 +4211,8 @@
       <c r="N33" t="s">
         <v>85</v>
       </c>
-      <c r="P33" s="3"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>514</v>
       </c>
@@ -4276,9 +4246,8 @@
       <c r="N34" t="s">
         <v>85</v>
       </c>
-      <c r="P34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>516</v>
       </c>
@@ -4312,9 +4281,8 @@
       <c r="N35" t="s">
         <v>85</v>
       </c>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>518</v>
       </c>
@@ -4348,9 +4316,8 @@
       <c r="N36" t="s">
         <v>85</v>
       </c>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>520</v>
       </c>
@@ -4384,9 +4351,8 @@
       <c r="N37" t="s">
         <v>85</v>
       </c>
-      <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>522</v>
       </c>
@@ -4420,9 +4386,8 @@
       <c r="N38" t="s">
         <v>85</v>
       </c>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>526</v>
       </c>
@@ -4456,9 +4421,8 @@
       <c r="N39" t="s">
         <v>85</v>
       </c>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>531</v>
       </c>
@@ -4498,9 +4462,8 @@
       <c r="N40" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>552</v>
       </c>
@@ -4534,9 +4497,8 @@
       <c r="N41" t="s">
         <v>85</v>
       </c>
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -4576,9 +4538,8 @@
       <c r="N42" t="s">
         <v>21</v>
       </c>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -4618,9 +4579,8 @@
       <c r="N43" t="s">
         <v>21</v>
       </c>
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>576</v>
       </c>
@@ -4660,9 +4620,8 @@
       <c r="N44" t="s">
         <v>21</v>
       </c>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>510</v>
       </c>
@@ -4705,9 +4664,8 @@
       <c r="N45" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="P45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>524</v>
       </c>
@@ -4744,15 +4702,14 @@
       <c r="L46" t="s">
         <v>85</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="N46" t="s">
         <v>21</v>
       </c>
-      <c r="P46" s="3"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>528</v>
       </c>
@@ -4795,9 +4752,8 @@
       <c r="N47" t="s">
         <v>21</v>
       </c>
-      <c r="P47" s="3"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>534</v>
       </c>
@@ -4837,9 +4793,8 @@
       <c r="N48" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="P48" s="3"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>537</v>
       </c>
@@ -4879,9 +4834,8 @@
       <c r="N49" t="s">
         <v>21</v>
       </c>
-      <c r="P49" s="3"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>540</v>
       </c>
@@ -4921,9 +4875,8 @@
       <c r="N50" t="s">
         <v>21</v>
       </c>
-      <c r="P50" s="3"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>543</v>
       </c>
@@ -4963,9 +4916,8 @@
       <c r="N51" t="s">
         <v>21</v>
       </c>
-      <c r="P51" s="3"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>546</v>
       </c>
@@ -5008,9 +4960,8 @@
       <c r="N52" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="P52" s="3"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>549</v>
       </c>
@@ -5053,9 +5004,8 @@
       <c r="N53" t="s">
         <v>21</v>
       </c>
-      <c r="P53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>638</v>
       </c>
@@ -5095,9 +5045,8 @@
       <c r="N54" t="s">
         <v>21</v>
       </c>
-      <c r="P54" s="3"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -5137,9 +5086,8 @@
       <c r="N55" t="s">
         <v>21</v>
       </c>
-      <c r="P55" s="3"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -5182,9 +5130,8 @@
       <c r="N56" t="s">
         <v>21</v>
       </c>
-      <c r="P56" s="3"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -5224,9 +5171,8 @@
       <c r="N57" t="s">
         <v>21</v>
       </c>
-      <c r="P57" s="3"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -5269,9 +5215,8 @@
       <c r="N58" t="s">
         <v>21</v>
       </c>
-      <c r="P58" s="3"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -5311,9 +5256,8 @@
       <c r="N59" t="s">
         <v>21</v>
       </c>
-      <c r="P59" s="3"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -5353,9 +5297,8 @@
       <c r="N60" t="s">
         <v>21</v>
       </c>
-      <c r="P60" s="3"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -5395,9 +5338,8 @@
       <c r="N61" t="s">
         <v>21</v>
       </c>
-      <c r="P61" s="3"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>105</v>
       </c>
@@ -5440,9 +5382,8 @@
       <c r="N62" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="P62" s="3"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>108</v>
       </c>
@@ -5482,9 +5423,8 @@
       <c r="N63" t="s">
         <v>21</v>
       </c>
-      <c r="P63" s="3"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -5524,9 +5464,8 @@
       <c r="N64" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P64" s="3"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>114</v>
       </c>
@@ -5566,9 +5505,8 @@
       <c r="N65" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="P65" s="3"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>117</v>
       </c>
@@ -5608,9 +5546,8 @@
       <c r="N66" t="s">
         <v>21</v>
       </c>
-      <c r="P66" s="3"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>119</v>
       </c>
@@ -5653,9 +5590,8 @@
       <c r="O67" t="s">
         <v>643</v>
       </c>
-      <c r="P67" s="3"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>204</v>
       </c>
@@ -5695,9 +5631,8 @@
       <c r="N68" t="s">
         <v>21</v>
       </c>
-      <c r="P68" s="3"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>400</v>
       </c>
@@ -5737,9 +5672,8 @@
       <c r="N69" t="s">
         <v>21</v>
       </c>
-      <c r="P69" s="3"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>592</v>
       </c>
@@ -5782,9 +5716,8 @@
       <c r="O70" t="s">
         <v>643</v>
       </c>
-      <c r="P70" s="3"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>596</v>
       </c>
@@ -5827,9 +5760,8 @@
       <c r="O71" t="s">
         <v>643</v>
       </c>
-      <c r="P71" s="3"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>417</v>
       </c>
@@ -5869,9 +5801,8 @@
       <c r="N72" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P72" s="3"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>123</v>
       </c>
@@ -5905,9 +5836,8 @@
       <c r="N73" t="s">
         <v>20</v>
       </c>
-      <c r="P73" s="3"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -5941,9 +5871,8 @@
       <c r="N74" t="s">
         <v>75</v>
       </c>
-      <c r="P74" s="3"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>572</v>
       </c>
@@ -5977,9 +5906,8 @@
       <c r="N75" t="s">
         <v>573</v>
       </c>
-      <c r="P75" s="3"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>38</v>
       </c>
@@ -6022,9 +5950,8 @@
       <c r="N76" t="s">
         <v>19</v>
       </c>
-      <c r="P76" s="3"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -6067,9 +5994,8 @@
       <c r="N77" t="s">
         <v>19</v>
       </c>
-      <c r="P77" s="3"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>170</v>
       </c>
@@ -6109,9 +6035,8 @@
       <c r="N78" t="s">
         <v>19</v>
       </c>
-      <c r="P78" s="3"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>173</v>
       </c>
@@ -6151,9 +6076,8 @@
       <c r="N79" t="s">
         <v>19</v>
       </c>
-      <c r="P79" s="3"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -6193,9 +6117,8 @@
       <c r="N80" t="s">
         <v>19</v>
       </c>
-      <c r="P80" s="3"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>187</v>
       </c>
@@ -6235,9 +6158,8 @@
       <c r="N81" t="s">
         <v>19</v>
       </c>
-      <c r="P81" s="3"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>191</v>
       </c>
@@ -6277,9 +6199,8 @@
       <c r="N82" t="s">
         <v>19</v>
       </c>
-      <c r="P82" s="3"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>194</v>
       </c>
@@ -6319,9 +6240,8 @@
       <c r="N83" t="s">
         <v>19</v>
       </c>
-      <c r="P83" s="3"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>198</v>
       </c>
@@ -6364,9 +6284,8 @@
       <c r="N84" t="s">
         <v>19</v>
       </c>
-      <c r="P84" s="3"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>201</v>
       </c>
@@ -6409,9 +6328,8 @@
       <c r="N85" t="s">
         <v>19</v>
       </c>
-      <c r="P85" s="3"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>208</v>
       </c>
@@ -6445,9 +6363,8 @@
       <c r="N86" t="s">
         <v>17</v>
       </c>
-      <c r="P86" s="3"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>210</v>
       </c>
@@ -6481,9 +6398,8 @@
       <c r="N87" t="s">
         <v>17</v>
       </c>
-      <c r="P87" s="3"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>212</v>
       </c>
@@ -6517,9 +6433,8 @@
       <c r="N88" t="s">
         <v>17</v>
       </c>
-      <c r="P88" s="3"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>214</v>
       </c>
@@ -6553,9 +6468,8 @@
       <c r="N89" t="s">
         <v>17</v>
       </c>
-      <c r="P89" s="3"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>216</v>
       </c>
@@ -6589,9 +6503,8 @@
       <c r="N90" t="s">
         <v>17</v>
       </c>
-      <c r="P90" s="3"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>218</v>
       </c>
@@ -6625,9 +6538,8 @@
       <c r="N91" t="s">
         <v>17</v>
       </c>
-      <c r="P91" s="3"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>220</v>
       </c>
@@ -6661,9 +6573,8 @@
       <c r="N92" t="s">
         <v>17</v>
       </c>
-      <c r="P92" s="3"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>222</v>
       </c>
@@ -6697,9 +6608,8 @@
       <c r="N93" t="s">
         <v>17</v>
       </c>
-      <c r="P93" s="3"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>224</v>
       </c>
@@ -6733,9 +6643,8 @@
       <c r="N94" t="s">
         <v>17</v>
       </c>
-      <c r="P94" s="3"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>226</v>
       </c>
@@ -6769,9 +6678,8 @@
       <c r="N95" t="s">
         <v>17</v>
       </c>
-      <c r="P95" s="3"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>228</v>
       </c>
@@ -6805,9 +6713,8 @@
       <c r="N96" t="s">
         <v>17</v>
       </c>
-      <c r="P96" s="3"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>230</v>
       </c>
@@ -6841,9 +6748,8 @@
       <c r="N97" t="s">
         <v>17</v>
       </c>
-      <c r="P97" s="3"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -6877,9 +6783,8 @@
       <c r="N98" t="s">
         <v>17</v>
       </c>
-      <c r="P98" s="3"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -6913,9 +6818,8 @@
       <c r="N99" t="s">
         <v>17</v>
       </c>
-      <c r="P99" s="3"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -6949,9 +6853,8 @@
       <c r="N100" t="s">
         <v>17</v>
       </c>
-      <c r="P100" s="3"/>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>238</v>
       </c>
@@ -6985,9 +6888,8 @@
       <c r="N101" t="s">
         <v>17</v>
       </c>
-      <c r="P101" s="3"/>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>240</v>
       </c>
@@ -7021,9 +6923,8 @@
       <c r="N102" t="s">
         <v>17</v>
       </c>
-      <c r="P102" s="3"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>242</v>
       </c>
@@ -7057,9 +6958,8 @@
       <c r="N103" t="s">
         <v>17</v>
       </c>
-      <c r="P103" s="3"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>244</v>
       </c>
@@ -7093,9 +6993,8 @@
       <c r="N104" t="s">
         <v>17</v>
       </c>
-      <c r="P104" s="3"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>246</v>
       </c>
@@ -7129,9 +7028,8 @@
       <c r="N105" t="s">
         <v>17</v>
       </c>
-      <c r="P105" s="3"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>248</v>
       </c>
@@ -7165,9 +7063,8 @@
       <c r="N106" t="s">
         <v>17</v>
       </c>
-      <c r="P106" s="3"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>250</v>
       </c>
@@ -7201,9 +7098,8 @@
       <c r="N107" t="s">
         <v>17</v>
       </c>
-      <c r="P107" s="3"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>252</v>
       </c>
@@ -7237,9 +7133,8 @@
       <c r="N108" t="s">
         <v>17</v>
       </c>
-      <c r="P108" s="3"/>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>254</v>
       </c>
@@ -7273,9 +7168,8 @@
       <c r="N109" t="s">
         <v>17</v>
       </c>
-      <c r="P109" s="3"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>256</v>
       </c>
@@ -7309,9 +7203,8 @@
       <c r="N110" t="s">
         <v>17</v>
       </c>
-      <c r="P110" s="3"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>258</v>
       </c>
@@ -7345,9 +7238,8 @@
       <c r="N111" t="s">
         <v>17</v>
       </c>
-      <c r="P111" s="3"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>260</v>
       </c>
@@ -7381,9 +7273,8 @@
       <c r="N112" t="s">
         <v>17</v>
       </c>
-      <c r="P112" s="3"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>262</v>
       </c>
@@ -7417,9 +7308,8 @@
       <c r="N113" t="s">
         <v>17</v>
       </c>
-      <c r="P113" s="3"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>264</v>
       </c>
@@ -7453,9 +7343,8 @@
       <c r="N114" t="s">
         <v>17</v>
       </c>
-      <c r="P114" s="3"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>266</v>
       </c>
@@ -7489,9 +7378,8 @@
       <c r="N115" t="s">
         <v>17</v>
       </c>
-      <c r="P115" s="3"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>268</v>
       </c>
@@ -7525,9 +7413,8 @@
       <c r="N116" t="s">
         <v>17</v>
       </c>
-      <c r="P116" s="3"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>270</v>
       </c>
@@ -7561,9 +7448,8 @@
       <c r="N117" t="s">
         <v>17</v>
       </c>
-      <c r="P117" s="3"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>272</v>
       </c>
@@ -7597,9 +7483,8 @@
       <c r="N118" t="s">
         <v>17</v>
       </c>
-      <c r="P118" s="3"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>274</v>
       </c>
@@ -7633,9 +7518,8 @@
       <c r="N119" t="s">
         <v>17</v>
       </c>
-      <c r="P119" s="3"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>276</v>
       </c>
@@ -7669,9 +7553,8 @@
       <c r="N120" t="s">
         <v>17</v>
       </c>
-      <c r="P120" s="3"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>278</v>
       </c>
@@ -7705,9 +7588,8 @@
       <c r="N121" t="s">
         <v>17</v>
       </c>
-      <c r="P121" s="3"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>280</v>
       </c>
@@ -7741,9 +7623,8 @@
       <c r="N122" t="s">
         <v>17</v>
       </c>
-      <c r="P122" s="3"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>282</v>
       </c>
@@ -7777,9 +7658,8 @@
       <c r="N123" t="s">
         <v>17</v>
       </c>
-      <c r="P123" s="3"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>284</v>
       </c>
@@ -7813,9 +7693,8 @@
       <c r="N124" t="s">
         <v>17</v>
       </c>
-      <c r="P124" s="3"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>286</v>
       </c>
@@ -7849,9 +7728,8 @@
       <c r="N125" t="s">
         <v>17</v>
       </c>
-      <c r="P125" s="3"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>288</v>
       </c>
@@ -7885,9 +7763,8 @@
       <c r="N126" t="s">
         <v>17</v>
       </c>
-      <c r="P126" s="3"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>290</v>
       </c>
@@ -7921,9 +7798,8 @@
       <c r="N127" t="s">
         <v>17</v>
       </c>
-      <c r="P127" s="3"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>292</v>
       </c>
@@ -7957,9 +7833,8 @@
       <c r="N128" t="s">
         <v>17</v>
       </c>
-      <c r="P128" s="3"/>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>294</v>
       </c>
@@ -7993,9 +7868,8 @@
       <c r="N129" t="s">
         <v>17</v>
       </c>
-      <c r="P129" s="3"/>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>296</v>
       </c>
@@ -8029,9 +7903,8 @@
       <c r="N130" t="s">
         <v>17</v>
       </c>
-      <c r="P130" s="3"/>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>298</v>
       </c>
@@ -8065,9 +7938,8 @@
       <c r="N131" t="s">
         <v>17</v>
       </c>
-      <c r="P131" s="3"/>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>300</v>
       </c>
@@ -8101,9 +7973,8 @@
       <c r="N132" t="s">
         <v>17</v>
       </c>
-      <c r="P132" s="3"/>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>302</v>
       </c>
@@ -8137,9 +8008,8 @@
       <c r="N133" t="s">
         <v>17</v>
       </c>
-      <c r="P133" s="3"/>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>304</v>
       </c>
@@ -8173,9 +8043,8 @@
       <c r="N134" t="s">
         <v>17</v>
       </c>
-      <c r="P134" s="3"/>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>306</v>
       </c>
@@ -8209,9 +8078,8 @@
       <c r="N135" t="s">
         <v>17</v>
       </c>
-      <c r="P135" s="3"/>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>308</v>
       </c>
@@ -8245,9 +8113,8 @@
       <c r="N136" t="s">
         <v>17</v>
       </c>
-      <c r="P136" s="3"/>
-    </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>310</v>
       </c>
@@ -8281,9 +8148,8 @@
       <c r="N137" t="s">
         <v>17</v>
       </c>
-      <c r="P137" s="3"/>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>312</v>
       </c>
@@ -8317,9 +8183,8 @@
       <c r="N138" t="s">
         <v>17</v>
       </c>
-      <c r="P138" s="3"/>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>314</v>
       </c>
@@ -8353,9 +8218,8 @@
       <c r="N139" t="s">
         <v>17</v>
       </c>
-      <c r="P139" s="3"/>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>316</v>
       </c>
@@ -8389,9 +8253,8 @@
       <c r="N140" t="s">
         <v>17</v>
       </c>
-      <c r="P140" s="3"/>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>318</v>
       </c>
@@ -8425,9 +8288,8 @@
       <c r="N141" t="s">
         <v>17</v>
       </c>
-      <c r="P141" s="3"/>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>320</v>
       </c>
@@ -8461,9 +8323,8 @@
       <c r="N142" t="s">
         <v>17</v>
       </c>
-      <c r="P142" s="3"/>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>322</v>
       </c>
@@ -8497,9 +8358,8 @@
       <c r="N143" t="s">
         <v>17</v>
       </c>
-      <c r="P143" s="3"/>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>324</v>
       </c>
@@ -8533,9 +8393,8 @@
       <c r="N144" t="s">
         <v>17</v>
       </c>
-      <c r="P144" s="3"/>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>326</v>
       </c>
@@ -8569,9 +8428,8 @@
       <c r="N145" t="s">
         <v>17</v>
       </c>
-      <c r="P145" s="3"/>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>328</v>
       </c>
@@ -8605,9 +8463,8 @@
       <c r="N146" t="s">
         <v>17</v>
       </c>
-      <c r="P146" s="3"/>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>330</v>
       </c>
@@ -8641,9 +8498,8 @@
       <c r="N147" t="s">
         <v>17</v>
       </c>
-      <c r="P147" s="3"/>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>332</v>
       </c>
@@ -8677,9 +8533,8 @@
       <c r="N148" t="s">
         <v>17</v>
       </c>
-      <c r="P148" s="3"/>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>334</v>
       </c>
@@ -8713,9 +8568,8 @@
       <c r="N149" t="s">
         <v>17</v>
       </c>
-      <c r="P149" s="3"/>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>336</v>
       </c>
@@ -8749,9 +8603,8 @@
       <c r="N150" t="s">
         <v>17</v>
       </c>
-      <c r="P150" s="3"/>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>338</v>
       </c>
@@ -8785,9 +8638,8 @@
       <c r="N151" t="s">
         <v>17</v>
       </c>
-      <c r="P151" s="3"/>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>340</v>
       </c>
@@ -8821,9 +8673,8 @@
       <c r="N152" t="s">
         <v>17</v>
       </c>
-      <c r="P152" s="3"/>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>342</v>
       </c>
@@ -8857,9 +8708,8 @@
       <c r="N153" t="s">
         <v>17</v>
       </c>
-      <c r="P153" s="3"/>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>344</v>
       </c>
@@ -8893,9 +8743,8 @@
       <c r="N154" t="s">
         <v>17</v>
       </c>
-      <c r="P154" s="3"/>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>346</v>
       </c>
@@ -8929,9 +8778,8 @@
       <c r="N155" t="s">
         <v>17</v>
       </c>
-      <c r="P155" s="3"/>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>348</v>
       </c>
@@ -8965,9 +8813,8 @@
       <c r="N156" t="s">
         <v>17</v>
       </c>
-      <c r="P156" s="3"/>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>350</v>
       </c>
@@ -9001,9 +8848,8 @@
       <c r="N157" t="s">
         <v>17</v>
       </c>
-      <c r="P157" s="3"/>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>352</v>
       </c>
@@ -9037,9 +8883,8 @@
       <c r="N158" t="s">
         <v>17</v>
       </c>
-      <c r="P158" s="3"/>
-    </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>354</v>
       </c>
@@ -9073,9 +8918,8 @@
       <c r="N159" t="s">
         <v>17</v>
       </c>
-      <c r="P159" s="3"/>
-    </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>356</v>
       </c>
@@ -9109,9 +8953,8 @@
       <c r="N160" t="s">
         <v>17</v>
       </c>
-      <c r="P160" s="3"/>
-    </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>358</v>
       </c>
@@ -9145,9 +8988,8 @@
       <c r="N161" t="s">
         <v>17</v>
       </c>
-      <c r="P161" s="3"/>
-    </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>360</v>
       </c>
@@ -9181,9 +9023,8 @@
       <c r="N162" t="s">
         <v>17</v>
       </c>
-      <c r="P162" s="3"/>
-    </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>362</v>
       </c>
@@ -9217,9 +9058,8 @@
       <c r="N163" t="s">
         <v>17</v>
       </c>
-      <c r="P163" s="3"/>
-    </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>364</v>
       </c>
@@ -9253,9 +9093,8 @@
       <c r="N164" t="s">
         <v>17</v>
       </c>
-      <c r="P164" s="3"/>
-    </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>366</v>
       </c>
@@ -9289,9 +9128,8 @@
       <c r="N165" t="s">
         <v>17</v>
       </c>
-      <c r="P165" s="3"/>
-    </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>368</v>
       </c>
@@ -9325,9 +9163,8 @@
       <c r="N166" t="s">
         <v>17</v>
       </c>
-      <c r="P166" s="3"/>
-    </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>370</v>
       </c>
@@ -9361,9 +9198,8 @@
       <c r="N167" t="s">
         <v>17</v>
       </c>
-      <c r="P167" s="3"/>
-    </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>372</v>
       </c>
@@ -9397,9 +9233,8 @@
       <c r="N168" t="s">
         <v>17</v>
       </c>
-      <c r="P168" s="3"/>
-    </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>374</v>
       </c>
@@ -9433,9 +9268,8 @@
       <c r="N169" t="s">
         <v>17</v>
       </c>
-      <c r="P169" s="3"/>
-    </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>376</v>
       </c>
@@ -9469,9 +9303,8 @@
       <c r="N170" t="s">
         <v>17</v>
       </c>
-      <c r="P170" s="3"/>
-    </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>378</v>
       </c>
@@ -9505,9 +9338,8 @@
       <c r="N171" t="s">
         <v>17</v>
       </c>
-      <c r="P171" s="3"/>
-    </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>380</v>
       </c>
@@ -9541,9 +9373,8 @@
       <c r="N172" t="s">
         <v>17</v>
       </c>
-      <c r="P172" s="3"/>
-    </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>382</v>
       </c>
@@ -9577,9 +9408,8 @@
       <c r="N173" t="s">
         <v>17</v>
       </c>
-      <c r="P173" s="3"/>
-    </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>384</v>
       </c>
@@ -9613,9 +9443,8 @@
       <c r="N174" t="s">
         <v>17</v>
       </c>
-      <c r="P174" s="3"/>
-    </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>386</v>
       </c>
@@ -9649,9 +9478,8 @@
       <c r="N175" t="s">
         <v>17</v>
       </c>
-      <c r="P175" s="3"/>
-    </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>388</v>
       </c>
@@ -9685,9 +9513,8 @@
       <c r="N176" t="s">
         <v>17</v>
       </c>
-      <c r="P176" s="3"/>
-    </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>390</v>
       </c>
@@ -9721,9 +9548,8 @@
       <c r="N177" t="s">
         <v>17</v>
       </c>
-      <c r="P177" s="3"/>
-    </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>392</v>
       </c>
@@ -9757,9 +9583,8 @@
       <c r="N178" t="s">
         <v>17</v>
       </c>
-      <c r="P178" s="3"/>
-    </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>394</v>
       </c>
@@ -9793,9 +9618,8 @@
       <c r="N179" t="s">
         <v>17</v>
       </c>
-      <c r="P179" s="3"/>
-    </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>396</v>
       </c>
@@ -9829,9 +9653,8 @@
       <c r="N180" t="s">
         <v>17</v>
       </c>
-      <c r="P180" s="3"/>
-    </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>398</v>
       </c>
@@ -9865,9 +9688,8 @@
       <c r="N181" t="s">
         <v>17</v>
       </c>
-      <c r="P181" s="3"/>
-    </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>562</v>
       </c>
@@ -9901,9 +9723,8 @@
       <c r="N182" t="s">
         <v>563</v>
       </c>
-      <c r="P182" s="3"/>
-    </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>407</v>
       </c>
@@ -9937,9 +9758,8 @@
       <c r="N183" t="s">
         <v>408</v>
       </c>
-      <c r="P183" s="3"/>
-    </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>608</v>
       </c>
@@ -9973,9 +9793,8 @@
       <c r="N184" t="s">
         <v>609</v>
       </c>
-      <c r="P184" s="3"/>
-    </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>611</v>
       </c>
@@ -10009,9 +9828,8 @@
       <c r="N185" t="s">
         <v>609</v>
       </c>
-      <c r="P185" s="3"/>
-    </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>613</v>
       </c>
@@ -10045,9 +9863,8 @@
       <c r="N186" t="s">
         <v>609</v>
       </c>
-      <c r="P186" s="3"/>
-    </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>615</v>
       </c>
@@ -10081,9 +9898,8 @@
       <c r="N187" t="s">
         <v>609</v>
       </c>
-      <c r="P187" s="3"/>
-    </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>617</v>
       </c>
@@ -10117,9 +9933,8 @@
       <c r="N188" t="s">
         <v>609</v>
       </c>
-      <c r="P188" s="3"/>
-    </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>619</v>
       </c>
@@ -10153,9 +9968,8 @@
       <c r="N189" t="s">
         <v>609</v>
       </c>
-      <c r="P189" s="3"/>
-    </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>428</v>
       </c>
@@ -10189,9 +10003,8 @@
       <c r="N190" t="s">
         <v>429</v>
       </c>
-      <c r="P190" s="3"/>
-    </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>432</v>
       </c>
@@ -10225,9 +10038,8 @@
       <c r="N191" t="s">
         <v>429</v>
       </c>
-      <c r="P191" s="3"/>
-    </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>434</v>
       </c>
@@ -10261,9 +10073,8 @@
       <c r="N192" t="s">
         <v>429</v>
       </c>
-      <c r="P192" s="3"/>
-    </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>175</v>
       </c>
@@ -10306,9 +10117,8 @@
       <c r="O193" t="s">
         <v>643</v>
       </c>
-      <c r="P193" s="3"/>
-    </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>423</v>
       </c>
@@ -10342,9 +10152,8 @@
       <c r="N194" t="s">
         <v>425</v>
       </c>
-      <c r="P194" s="3"/>
-    </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>436</v>
       </c>
@@ -10378,9 +10187,8 @@
       <c r="N195" t="s">
         <v>178</v>
       </c>
-      <c r="P195" s="3"/>
-    </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>438</v>
       </c>
@@ -10414,9 +10222,8 @@
       <c r="N196" t="s">
         <v>178</v>
       </c>
-      <c r="P196" s="3"/>
-    </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>605</v>
       </c>
@@ -10450,9 +10257,8 @@
       <c r="N197" t="s">
         <v>606</v>
       </c>
-      <c r="P197" s="3"/>
-    </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>125</v>
       </c>
@@ -10492,9 +10298,8 @@
       <c r="O198" t="s">
         <v>643</v>
       </c>
-      <c r="P198" s="3"/>
-    </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>405</v>
       </c>
@@ -10528,9 +10333,8 @@
       <c r="N199" t="s">
         <v>404</v>
       </c>
-      <c r="P199" s="3"/>
-    </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>410</v>
       </c>
@@ -10564,9 +10368,8 @@
       <c r="N200" t="s">
         <v>411</v>
       </c>
-      <c r="P200" s="3"/>
-    </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>420</v>
       </c>
@@ -10600,9 +10403,8 @@
       <c r="N201" t="s">
         <v>421</v>
       </c>
-      <c r="P201" s="3"/>
-    </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>440</v>
       </c>
@@ -10636,9 +10438,8 @@
       <c r="N202" t="s">
         <v>441</v>
       </c>
-      <c r="P202" s="3"/>
-    </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>443</v>
       </c>
@@ -10672,9 +10473,8 @@
       <c r="N203" t="s">
         <v>441</v>
       </c>
-      <c r="P203" s="3"/>
-    </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>445</v>
       </c>
@@ -10708,9 +10508,8 @@
       <c r="N204" t="s">
         <v>441</v>
       </c>
-      <c r="P204" s="3"/>
-    </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>447</v>
       </c>
@@ -10744,9 +10543,8 @@
       <c r="N205" t="s">
         <v>441</v>
       </c>
-      <c r="P205" s="3"/>
-    </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>449</v>
       </c>
@@ -10780,9 +10578,8 @@
       <c r="N206" t="s">
         <v>441</v>
       </c>
-      <c r="P206" s="3"/>
-    </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>451</v>
       </c>
@@ -10816,9 +10613,8 @@
       <c r="N207" t="s">
         <v>441</v>
       </c>
-      <c r="P207" s="3"/>
-    </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>453</v>
       </c>
@@ -10852,9 +10648,8 @@
       <c r="N208" t="s">
         <v>441</v>
       </c>
-      <c r="P208" s="3"/>
-    </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>455</v>
       </c>
@@ -10888,9 +10683,8 @@
       <c r="N209" t="s">
         <v>441</v>
       </c>
-      <c r="P209" s="3"/>
-    </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>459</v>
       </c>
@@ -10924,9 +10718,8 @@
       <c r="N210" t="s">
         <v>441</v>
       </c>
-      <c r="P210" s="3"/>
-    </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>461</v>
       </c>
@@ -10960,9 +10753,8 @@
       <c r="N211" t="s">
         <v>441</v>
       </c>
-      <c r="P211" s="3"/>
-    </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>463</v>
       </c>
@@ -10996,9 +10788,8 @@
       <c r="N212" t="s">
         <v>441</v>
       </c>
-      <c r="P212" s="3"/>
-    </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>465</v>
       </c>
@@ -11032,9 +10823,8 @@
       <c r="N213" t="s">
         <v>441</v>
       </c>
-      <c r="P213" s="3"/>
-    </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>467</v>
       </c>
@@ -11068,9 +10858,8 @@
       <c r="N214" t="s">
         <v>441</v>
       </c>
-      <c r="P214" s="3"/>
-    </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>469</v>
       </c>
@@ -11104,9 +10893,8 @@
       <c r="N215" t="s">
         <v>441</v>
       </c>
-      <c r="P215" s="3"/>
-    </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>471</v>
       </c>
@@ -11140,9 +10928,8 @@
       <c r="N216" t="s">
         <v>441</v>
       </c>
-      <c r="P216" s="3"/>
-    </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>473</v>
       </c>
@@ -11176,9 +10963,8 @@
       <c r="N217" t="s">
         <v>441</v>
       </c>
-      <c r="P217" s="3"/>
-    </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>475</v>
       </c>
@@ -11212,9 +10998,8 @@
       <c r="N218" t="s">
         <v>441</v>
       </c>
-      <c r="P218" s="3"/>
-    </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>477</v>
       </c>
@@ -11248,9 +11033,8 @@
       <c r="N219" t="s">
         <v>441</v>
       </c>
-      <c r="P219" s="3"/>
-    </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>479</v>
       </c>
@@ -11284,9 +11068,8 @@
       <c r="N220" t="s">
         <v>441</v>
       </c>
-      <c r="P220" s="3"/>
-    </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>481</v>
       </c>
@@ -11320,9 +11103,8 @@
       <c r="N221" t="s">
         <v>441</v>
       </c>
-      <c r="P221" s="3"/>
-    </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>483</v>
       </c>
@@ -11356,9 +11138,8 @@
       <c r="N222" t="s">
         <v>441</v>
       </c>
-      <c r="P222" s="3"/>
-    </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>485</v>
       </c>
@@ -11392,9 +11173,8 @@
       <c r="N223" t="s">
         <v>441</v>
       </c>
-      <c r="P223" s="3"/>
-    </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>487</v>
       </c>
@@ -11428,9 +11208,8 @@
       <c r="N224" t="s">
         <v>441</v>
       </c>
-      <c r="P224" s="3"/>
-    </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>489</v>
       </c>
@@ -11464,9 +11243,8 @@
       <c r="N225" t="s">
         <v>441</v>
       </c>
-      <c r="P225" s="3"/>
-    </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>491</v>
       </c>
@@ -11500,9 +11278,8 @@
       <c r="N226" t="s">
         <v>441</v>
       </c>
-      <c r="P226" s="3"/>
-    </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>493</v>
       </c>
@@ -11536,9 +11313,8 @@
       <c r="N227" t="s">
         <v>441</v>
       </c>
-      <c r="P227" s="3"/>
-    </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>495</v>
       </c>
@@ -11572,9 +11348,8 @@
       <c r="N228" t="s">
         <v>441</v>
       </c>
-      <c r="P228" s="3"/>
-    </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>497</v>
       </c>
@@ -11608,9 +11383,8 @@
       <c r="N229" t="s">
         <v>441</v>
       </c>
-      <c r="P229" s="3"/>
-    </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>499</v>
       </c>
@@ -11644,9 +11418,8 @@
       <c r="N230" t="s">
         <v>441</v>
       </c>
-      <c r="P230" s="3"/>
-    </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>501</v>
       </c>
@@ -11680,9 +11453,8 @@
       <c r="N231" t="s">
         <v>441</v>
       </c>
-      <c r="P231" s="3"/>
-    </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>566</v>
       </c>
@@ -11716,9 +11488,8 @@
       <c r="N232" t="s">
         <v>567</v>
       </c>
-      <c r="P232" s="3"/>
-    </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>569</v>
       </c>
@@ -11752,9 +11523,8 @@
       <c r="N233" t="s">
         <v>570</v>
       </c>
-      <c r="P233" s="3"/>
-    </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>579</v>
       </c>
@@ -11788,9 +11558,8 @@
       <c r="N234" t="s">
         <v>580</v>
       </c>
-      <c r="P234" s="3"/>
-    </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>582</v>
       </c>
@@ -11824,9 +11593,8 @@
       <c r="N235" t="s">
         <v>580</v>
       </c>
-      <c r="P235" s="3"/>
-    </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>584</v>
       </c>
@@ -11860,9 +11628,8 @@
       <c r="N236" t="s">
         <v>580</v>
       </c>
-      <c r="P236" s="3"/>
-    </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>586</v>
       </c>
@@ -11896,9 +11663,8 @@
       <c r="N237" t="s">
         <v>580</v>
       </c>
-      <c r="P237" s="3"/>
-    </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>598</v>
       </c>
@@ -11932,9 +11698,8 @@
       <c r="N238" t="s">
         <v>599</v>
       </c>
-      <c r="P238" s="3"/>
-    </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>601</v>
       </c>
@@ -11980,9 +11745,8 @@
       <c r="O239" t="s">
         <v>643</v>
       </c>
-      <c r="P239" s="3"/>
-    </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>183</v>
       </c>
@@ -12016,9 +11780,8 @@
       <c r="N240" t="s">
         <v>18</v>
       </c>
-      <c r="P240" s="3"/>
-    </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>185</v>
       </c>
@@ -12052,9 +11815,8 @@
       <c r="N241" t="s">
         <v>18</v>
       </c>
-      <c r="P241" s="3"/>
-    </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>554</v>
       </c>
@@ -12088,9 +11850,8 @@
       <c r="N242" t="s">
         <v>18</v>
       </c>
-      <c r="P242" s="3"/>
-    </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>556</v>
       </c>
@@ -12124,9 +11885,8 @@
       <c r="N243" t="s">
         <v>18</v>
       </c>
-      <c r="P243" s="3"/>
-    </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>558</v>
       </c>
@@ -12160,9 +11920,8 @@
       <c r="N244" t="s">
         <v>18</v>
       </c>
-      <c r="P244" s="3"/>
-    </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>560</v>
       </c>
@@ -12196,9 +11955,8 @@
       <c r="N245" t="s">
         <v>18</v>
       </c>
-      <c r="P245" s="3"/>
-    </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>58</v>
       </c>
@@ -12241,9 +11999,8 @@
       <c r="O246" t="s">
         <v>643</v>
       </c>
-      <c r="P246" s="3"/>
-    </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>63</v>
       </c>
@@ -12277,9 +12034,8 @@
       <c r="N247" t="s">
         <v>61</v>
       </c>
-      <c r="P247" s="3"/>
-    </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>65</v>
       </c>
@@ -12313,9 +12069,8 @@
       <c r="N248" t="s">
         <v>61</v>
       </c>
-      <c r="P248" s="3"/>
-    </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>67</v>
       </c>
@@ -12349,9 +12104,8 @@
       <c r="N249" t="s">
         <v>61</v>
       </c>
-      <c r="P249" s="3"/>
-    </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>69</v>
       </c>
@@ -12385,9 +12139,8 @@
       <c r="N250" t="s">
         <v>61</v>
       </c>
-      <c r="P250" s="3"/>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>71</v>
       </c>
@@ -12421,9 +12174,8 @@
       <c r="N251" t="s">
         <v>61</v>
       </c>
-      <c r="P251" s="3"/>
-    </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>413</v>
       </c>
@@ -12466,9 +12218,8 @@
       <c r="O252" t="s">
         <v>643</v>
       </c>
-      <c r="P252" s="3"/>
-    </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>588</v>
       </c>
@@ -12502,9 +12253,8 @@
       <c r="N253" t="s">
         <v>589</v>
       </c>
-      <c r="P253" s="3"/>
-    </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>621</v>
       </c>
@@ -12538,9 +12288,8 @@
       <c r="N254" t="s">
         <v>622</v>
       </c>
-      <c r="P254" s="3"/>
-    </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>624</v>
       </c>
@@ -12574,9 +12323,8 @@
       <c r="N255" t="s">
         <v>622</v>
       </c>
-      <c r="P255" s="3"/>
-    </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>626</v>
       </c>
@@ -12610,9 +12358,8 @@
       <c r="N256" t="s">
         <v>622</v>
       </c>
-      <c r="P256" s="3"/>
-    </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>628</v>
       </c>
@@ -12646,9 +12393,8 @@
       <c r="N257" t="s">
         <v>622</v>
       </c>
-      <c r="P257" s="3"/>
-    </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>630</v>
       </c>
@@ -12682,9 +12428,8 @@
       <c r="N258" t="s">
         <v>622</v>
       </c>
-      <c r="P258" s="3"/>
-    </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>632</v>
       </c>
@@ -12718,9 +12463,8 @@
       <c r="N259" t="s">
         <v>622</v>
       </c>
-      <c r="P259" s="3"/>
-    </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>634</v>
       </c>
@@ -12754,9 +12498,8 @@
       <c r="N260" t="s">
         <v>622</v>
       </c>
-      <c r="P260" s="3"/>
-    </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>636</v>
       </c>
@@ -12790,13 +12533,6 @@
       <c r="N261" t="s">
         <v>622</v>
       </c>
-      <c r="P261" s="3"/>
-    </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P262" s="3"/>
-    </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P263" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O261">

</xml_diff>